<commit_message>
Sept 24 SSP updates
</commit_message>
<xml_diff>
--- a/tutorial/dac_scenarios/SSPs/_Diff.xlsx
+++ b/tutorial/dac_scenarios/SSPs/_Diff.xlsx
@@ -506,500 +506,461 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="P2">
-        <v>37.83602619118392</v>
-      </c>
       <c r="Q2">
-        <v>-1.730505228455741</v>
+        <v>34.69638015858982</v>
       </c>
       <c r="R2">
-        <v>-71.12743661288778</v>
+        <v>-26.9389830298353</v>
       </c>
       <c r="S2">
-        <v>-191.3116246141403</v>
+        <v>-146.4574609384943</v>
       </c>
       <c r="T2">
-        <v>-313.757231712573</v>
+        <v>-283.8968469856518</v>
       </c>
       <c r="U2">
-        <v>-424.2738594284331</v>
+        <v>-391.1227627719198</v>
       </c>
       <c r="V2">
-        <v>-539.5633162375466</v>
+        <v>-490.519535797212</v>
       </c>
       <c r="W2">
-        <v>-872.2166039740928</v>
+        <v>-812.332694417669</v>
       </c>
       <c r="X2">
-        <v>-919.7899702416487</v>
+        <v>-723.1289987016471</v>
       </c>
       <c r="Y2">
-        <v>-760.9449901748242</v>
+        <v>-1996.256981084404</v>
       </c>
       <c r="Z2">
-        <v>-797.630860611368</v>
+        <v>-1910.469919733242</v>
       </c>
       <c r="AA2">
-        <v>-703.2358416036047</v>
+        <v>-1201.69277056063</v>
       </c>
     </row>
     <row r="3" spans="1:27">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="P3">
-        <v>111.5905600431488</v>
-      </c>
       <c r="Q3">
-        <v>156.5870863189102</v>
+        <v>-171.8816458255606</v>
       </c>
       <c r="R3">
-        <v>138.2570719216128</v>
+        <v>-766.8029417826619</v>
       </c>
       <c r="S3">
-        <v>160.0163932840669</v>
+        <v>-985.1894092423827</v>
       </c>
       <c r="T3">
-        <v>235.727812115696</v>
+        <v>-1057.891732932264</v>
       </c>
       <c r="U3">
-        <v>165.571740793469</v>
+        <v>-996.3330636358082</v>
       </c>
       <c r="V3">
-        <v>-151.1962341576864</v>
+        <v>-1186.972913996136</v>
       </c>
       <c r="W3">
-        <v>-714.3310080375722</v>
+        <v>-2465.199073890797</v>
       </c>
       <c r="X3">
-        <v>-1237.820870540789</v>
+        <v>-3291.656942142021</v>
       </c>
       <c r="Y3">
-        <v>-1071.2170833372</v>
+        <v>-2851.813327760527</v>
       </c>
       <c r="Z3">
-        <v>-399.8450618551065</v>
+        <v>-1963.862416315807</v>
       </c>
       <c r="AA3">
-        <v>539.4362727069392</v>
+        <v>-1691.236984979456</v>
       </c>
     </row>
     <row r="4" spans="1:27">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="P4">
-        <v>30.54275144507005</v>
-      </c>
       <c r="Q4">
-        <v>25.24491557669194</v>
+        <v>7.431200764599907</v>
       </c>
       <c r="R4">
-        <v>4.499528132936689</v>
+        <v>-22.02977117085794</v>
       </c>
       <c r="S4">
-        <v>-4.934227109942356</v>
+        <v>-83.11760065520056</v>
       </c>
       <c r="T4">
-        <v>-37.46769161812307</v>
+        <v>-147.6054858712574</v>
       </c>
       <c r="U4">
-        <v>-76.8294955380664</v>
+        <v>-220.7351165972183</v>
       </c>
       <c r="V4">
-        <v>-121.7938105679553</v>
+        <v>-303.7603590478333</v>
       </c>
       <c r="W4">
-        <v>-101.574619820632</v>
+        <v>-657.7990617456937</v>
       </c>
       <c r="X4">
-        <v>-23.33353338979845</v>
+        <v>-1091.420065494662</v>
       </c>
       <c r="Y4">
-        <v>-12.64981682927362</v>
+        <v>-877.1508935295822</v>
       </c>
       <c r="Z4">
-        <v>-4.228033219616464</v>
+        <v>-811.5433269917892</v>
       </c>
       <c r="AA4">
-        <v>20.60273999454211</v>
+        <v>-351.0280795903536</v>
       </c>
     </row>
     <row r="5" spans="1:27">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="P5">
-        <v>49.67661615889892</v>
-      </c>
       <c r="Q5">
-        <v>40.55235821991437</v>
+        <v>45.88772144876566</v>
       </c>
       <c r="R5">
-        <v>1.092497534152699</v>
+        <v>-0.5035406081292422</v>
       </c>
       <c r="S5">
-        <v>-70.70185898194859</v>
+        <v>-42.08509019622556</v>
       </c>
       <c r="T5">
-        <v>-143.9621581439553</v>
+        <v>-80.04191050949044</v>
       </c>
       <c r="U5">
-        <v>-206.2834183494277</v>
+        <v>-153.1955808062492</v>
       </c>
       <c r="V5">
-        <v>-264.0135844115898</v>
+        <v>-243.903702765754</v>
       </c>
       <c r="W5">
-        <v>-470.5545808156759</v>
+        <v>-623.9250360012662</v>
       </c>
       <c r="X5">
-        <v>-811.5972063102254</v>
+        <v>-1482.857243862202</v>
       </c>
       <c r="Y5">
-        <v>-1196.789929374755</v>
+        <v>-1729.78595086159</v>
       </c>
       <c r="Z5">
-        <v>-1762.026568845862</v>
+        <v>-2647.891347494049</v>
       </c>
       <c r="AA5">
-        <v>-1455.1151587847</v>
+        <v>-5759.994447360386</v>
       </c>
     </row>
     <row r="6" spans="1:27">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="P6">
-        <v>67.46814107092518</v>
-      </c>
       <c r="Q6">
-        <v>42.3758922554639</v>
+        <v>63.18027215502912</v>
       </c>
       <c r="R6">
-        <v>-31.81229875845929</v>
+        <v>-7.070858447161299</v>
       </c>
       <c r="S6">
-        <v>-134.7534371487575</v>
+        <v>-73.50938246215605</v>
       </c>
       <c r="T6">
-        <v>-282.0983055782156</v>
+        <v>-231.3563518091696</v>
       </c>
       <c r="U6">
-        <v>-462.4559347821134</v>
+        <v>-354.1100394266708</v>
       </c>
       <c r="V6">
-        <v>-595.9251416112705</v>
+        <v>-420.3176936272977</v>
       </c>
       <c r="W6">
-        <v>-974.7650731035474</v>
+        <v>-889.3360357633879</v>
       </c>
       <c r="X6">
-        <v>-1402.515391838786</v>
+        <v>-2733.081710337864</v>
       </c>
       <c r="Y6">
-        <v>-1565.977247795894</v>
+        <v>-3632.92547371078</v>
       </c>
       <c r="Z6">
-        <v>-2009.377119101766</v>
+        <v>-6787.655561917422</v>
       </c>
       <c r="AA6">
-        <v>-3095.749408483165</v>
+        <v>-13135.84495522096</v>
       </c>
     </row>
     <row r="7" spans="1:27">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="P7">
-        <v>167.0912547866915</v>
-      </c>
       <c r="Q7">
-        <v>177.4475754137784</v>
+        <v>109.3333343292943</v>
       </c>
       <c r="R7">
-        <v>123.0581331914173</v>
+        <v>-55.70858328534996</v>
       </c>
       <c r="S7">
-        <v>-24.4802913090889</v>
+        <v>-160.4280375032772</v>
       </c>
       <c r="T7">
-        <v>-256.6507635630346</v>
+        <v>-254.4253579441036</v>
       </c>
       <c r="U7">
-        <v>-361.5343820443773</v>
+        <v>-340.1986459188897</v>
       </c>
       <c r="V7">
-        <v>-469.2652073436616</v>
+        <v>-469.664857884751</v>
       </c>
       <c r="W7">
-        <v>-706.3195234499362</v>
+        <v>-851.0965359428355</v>
       </c>
       <c r="X7">
-        <v>-1211.674646849037</v>
+        <v>-1073.533883216317</v>
       </c>
       <c r="Y7">
-        <v>-1581.922641979787</v>
+        <v>-646.3702680292732</v>
       </c>
       <c r="Z7">
-        <v>-2493.427985153378</v>
+        <v>-289.2864647605688</v>
       </c>
       <c r="AA7">
-        <v>-3293.066492819772</v>
+        <v>85.19946350476607</v>
       </c>
     </row>
     <row r="8" spans="1:27">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="P8">
-        <v>305.6098931426786</v>
-      </c>
       <c r="Q8">
-        <v>225.5378908402927</v>
+        <v>123.7520147028954</v>
       </c>
       <c r="R8">
-        <v>124.6651198823329</v>
+        <v>18.55221283122182</v>
       </c>
       <c r="S8">
-        <v>33.7395669936659</v>
+        <v>-68.27148455082533</v>
       </c>
       <c r="T8">
-        <v>-71.39023738720743</v>
+        <v>-177.5502885604708</v>
       </c>
       <c r="U8">
-        <v>-201.5468749447277</v>
+        <v>-309.8990866258553</v>
       </c>
       <c r="V8">
-        <v>-294.2504463975997</v>
+        <v>-543.8861411260295</v>
       </c>
       <c r="W8">
-        <v>-498.9688968745202</v>
+        <v>-1944.171021147397</v>
       </c>
       <c r="X8">
-        <v>-857.0974433947849</v>
+        <v>-6798.230133646563</v>
       </c>
       <c r="Y8">
-        <v>-1111.876422107762</v>
+        <v>-6723.593926639877</v>
       </c>
       <c r="Z8">
-        <v>-1222.457669369715</v>
+        <v>-6060.89959787308</v>
       </c>
       <c r="AA8">
-        <v>-1681.168903902413</v>
+        <v>-1220.18463416079</v>
       </c>
     </row>
     <row r="9" spans="1:27">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="P9">
-        <v>37.0134153902402</v>
-      </c>
       <c r="Q9">
-        <v>23.15835783769876</v>
+        <v>38.17585913825769</v>
       </c>
       <c r="R9">
-        <v>-12.26769229615286</v>
+        <v>-8.183226591304901</v>
       </c>
       <c r="S9">
-        <v>-51.09499763610381</v>
+        <v>-48.8635156627721</v>
       </c>
       <c r="T9">
-        <v>-99.15635790082717</v>
+        <v>-105.6351269118392</v>
       </c>
       <c r="U9">
-        <v>-149.1294657034405</v>
+        <v>-174.7068081505758</v>
       </c>
       <c r="V9">
-        <v>-201.4363446810953</v>
+        <v>-236.5809447984768</v>
       </c>
       <c r="W9">
-        <v>-462.335495152859</v>
+        <v>-722.7311709081712</v>
       </c>
       <c r="X9">
-        <v>-494.9242437576689</v>
+        <v>-1604.281185181418</v>
       </c>
       <c r="Y9">
-        <v>-336.0250934023545</v>
+        <v>-1455.67777630344</v>
       </c>
       <c r="Z9">
-        <v>-248.3989304357986</v>
+        <v>-1246.170272489308</v>
       </c>
       <c r="AA9">
-        <v>-332.8143132215925</v>
+        <v>-354.1848721814411</v>
       </c>
     </row>
     <row r="10" spans="1:27">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="P10">
-        <v>26.357925277503</v>
-      </c>
       <c r="Q10">
-        <v>-16.91878928890037</v>
+        <v>-20.99015300688166</v>
       </c>
       <c r="R10">
-        <v>-63.4503384752843</v>
+        <v>-112.3516688555226</v>
       </c>
       <c r="S10">
-        <v>-151.5744679763175</v>
+        <v>-200.2629971996486</v>
       </c>
       <c r="T10">
-        <v>-234.5600658587412</v>
+        <v>-299.1664186074325</v>
       </c>
       <c r="U10">
-        <v>-405.5037310960447</v>
+        <v>-405.0147993466621</v>
       </c>
       <c r="V10">
-        <v>-506.8849705024102</v>
+        <v>-513.6682477290864</v>
       </c>
       <c r="W10">
-        <v>-746.0007699837232</v>
+        <v>-1023.483919056334</v>
       </c>
       <c r="X10">
-        <v>-821.9946562625944</v>
+        <v>-1528.595673540802</v>
       </c>
       <c r="Y10">
-        <v>-752.1340726483859</v>
+        <v>-1169.824334542595</v>
       </c>
       <c r="Z10">
-        <v>-434.7294154307895</v>
+        <v>-995.1323565447985</v>
       </c>
       <c r="AA10">
-        <v>-89.88155640148261</v>
+        <v>-790.8226253271453</v>
       </c>
     </row>
     <row r="11" spans="1:27">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="P11">
-        <v>1.754296210929056</v>
-      </c>
       <c r="Q11">
-        <v>5.275371333032467</v>
+        <v>16.00300714702496</v>
       </c>
       <c r="R11">
-        <v>16.21094357753418</v>
+        <v>9.960796898525302</v>
       </c>
       <c r="S11">
-        <v>28.70165891298956</v>
+        <v>-34.05020768249531</v>
       </c>
       <c r="T11">
-        <v>-9.829507782865107</v>
+        <v>-90.99952318390088</v>
       </c>
       <c r="U11">
-        <v>-28.16714701785304</v>
+        <v>-167.6304709175562</v>
       </c>
       <c r="V11">
-        <v>-70.97721389933753</v>
+        <v>-344.6622603192554</v>
       </c>
       <c r="W11">
-        <v>-164.3850668193442</v>
+        <v>-1570.373584514152</v>
       </c>
       <c r="X11">
-        <v>-130.4048489874525</v>
+        <v>-4925.14461820703</v>
       </c>
       <c r="Y11">
-        <v>-9.637268003221379</v>
+        <v>-4558.038925791524</v>
       </c>
       <c r="Z11">
-        <v>-17.68453026336283</v>
+        <v>-3394.863172406475</v>
       </c>
       <c r="AA11">
-        <v>-24.33287506467047</v>
+        <v>-2088.653241936828</v>
       </c>
     </row>
     <row r="12" spans="1:27">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="P12">
-        <v>26.51778174222</v>
-      </c>
       <c r="Q12">
-        <v>9.658401755280011</v>
+        <v>-77.89775068598692</v>
       </c>
       <c r="R12">
-        <v>-16.64558135715106</v>
+        <v>-236.5379925745895</v>
       </c>
       <c r="S12">
-        <v>-62.42746055638872</v>
+        <v>-457.4003502513031</v>
       </c>
       <c r="T12">
-        <v>-93.98209601047847</v>
+        <v>-665.2581465679891</v>
       </c>
       <c r="U12">
-        <v>-197.7640623722232</v>
+        <v>-749.7447725900686</v>
       </c>
       <c r="V12">
-        <v>-257.8578271744341</v>
+        <v>-815.8900747733443</v>
       </c>
       <c r="W12">
-        <v>-398.4274905830528</v>
+        <v>-1145.674765810396</v>
       </c>
       <c r="X12">
-        <v>-244.3852024479129</v>
+        <v>-685.4746981795565</v>
       </c>
       <c r="Y12">
-        <v>48.27867006365614</v>
+        <v>-698.0676880510742</v>
       </c>
       <c r="Z12">
-        <v>-40.67650989536287</v>
+        <v>-1005.934822344592</v>
       </c>
       <c r="AA12">
-        <v>37.96224055580933</v>
+        <v>-674.5117732418621</v>
       </c>
     </row>
     <row r="13" spans="1:27">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="P13">
-        <v>91.04711499305449</v>
-      </c>
       <c r="Q13">
-        <v>54.93641635418317</v>
+        <v>28.91629080955727</v>
       </c>
       <c r="R13">
-        <v>40.47067648764778</v>
+        <v>-35.18547274014122</v>
       </c>
       <c r="S13">
-        <v>-14.79946397382355</v>
+        <v>-143.5563513469347</v>
       </c>
       <c r="T13">
-        <v>-120.3164918680905</v>
+        <v>-284.5316668555723</v>
       </c>
       <c r="U13">
-        <v>-212.5547026660038</v>
+        <v>-427.1915298542483</v>
       </c>
       <c r="V13">
-        <v>-302.4674472047238</v>
+        <v>-668.068460830879</v>
       </c>
       <c r="W13">
-        <v>-620.2007341717824</v>
+        <v>-1829.924452021452</v>
       </c>
       <c r="X13">
-        <v>-674.5531013812505</v>
+        <v>-4647.406677756597</v>
       </c>
       <c r="Y13">
-        <v>-686.1380060198112</v>
+        <v>-4184.342536970316</v>
       </c>
       <c r="Z13">
-        <v>-409.0171477383097</v>
+        <v>-3447.4636345431</v>
       </c>
       <c r="AA13">
-        <v>102.2229777489977</v>
+        <v>-768.4357733647569</v>
       </c>
     </row>
     <row r="14" spans="1:27">
       <c r="A14" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="P14">
-        <v>0</v>
       </c>
       <c r="Q14">
         <v>0</v>

</xml_diff>